<commit_message>
Ajout de quelques risques
</commit_message>
<xml_diff>
--- a/Rendu/AF/Analyse_risques.xlsx
+++ b/Rendu/AF/Analyse_risques.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badr\Documents\prt-ge-s2-2015-svn\trunk\Rendu\AF\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>N°</t>
   </si>
@@ -168,6 +163,21 @@
   </si>
   <si>
     <t>Faire une demande spéciale pour accéder à de meilleurs équipements</t>
+  </si>
+  <si>
+    <t>Revoir le cahier de charges</t>
+  </si>
+  <si>
+    <t>Temps de mise en œuvre prévue d'une fonctionnalité logicielle trop élevée</t>
+  </si>
+  <si>
+    <t>Douglas R.</t>
+  </si>
+  <si>
+    <t>Problèmes inattendus à débogger</t>
+  </si>
+  <si>
+    <t>Revoir le Gantt et allouer plus de temps au déboggage</t>
   </si>
 </sst>
 </file>
@@ -213,9 +223,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -223,6 +230,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -504,13 +514,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
@@ -547,18 +557,18 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -573,7 +583,7 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
@@ -581,18 +591,18 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -607,7 +617,7 @@
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H5" t="s">
@@ -627,7 +637,7 @@
       <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
@@ -647,7 +657,7 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
@@ -667,7 +677,7 @@
       <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H8" t="s">
@@ -675,222 +685,262 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
         <v>15</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>15</v>
       </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="6" t="s">
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C19" s="3">
         <v>3</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D19" s="3">
         <v>15</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="7" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H19" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>3</v>
       </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
         <v>15</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F22" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H22" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="F18:H18"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>